<commit_message>
Perbaikan Antrian Device Presensi
</commit_message>
<xml_diff>
--- a/pantauclient/media/temp_reports/Laporan_9A_2025-11-25.xlsx
+++ b/pantauclient/media/temp_reports/Laporan_9A_2025-11-25.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Sakit</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Izin</t>
+          <t>Hadir</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Hadir</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Sakit</t>
+          <t>Hadir</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
@@ -1302,21 +1302,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Hadir: 29</t>
+          <t>Hadir: 32</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Izin: 1</t>
+          <t>Izin: 0</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sakit: 2</t>
+          <t>Sakit: 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatis Kirim Database Tanpa Pencet SIMPAN
</commit_message>
<xml_diff>
--- a/pantauclient/media/temp_reports/Laporan_9A_2025-11-25.xlsx
+++ b/pantauclient/media/temp_reports/Laporan_9A_2025-11-25.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Hadir</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>Hadir</t>
+          <t>Sakit</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Hadir</t>
+          <t>Izin</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>Hadir</t>
+          <t>Izin</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>Hadir</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
@@ -1302,21 +1302,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Hadir: 32</t>
+          <t>Hadir: 29</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Izin: 0</t>
+          <t>Izin: 2</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sakit: 0</t>
+          <t>Sakit: 1</t>
         </is>
       </c>
     </row>

</xml_diff>